<commit_message>
Updated work protocol & distribution
</commit_message>
<xml_diff>
--- a/work_distribution/Nisslmueller_work_protocol_MS2.xlsx
+++ b/work_distribution/Nisslmueller_work_protocol_MS2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\utzn\Google Drive\Uni Wien\WS 2018-19\ISE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\utzn\Google Drive\Uni Wien\WS 2018-19\ISE\Projekt\Kino_JDBC\work_distribution\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{96208F11-58B3-47F4-8725-B372362994A5}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{7F2FD998-B779-4FFC-84A7-8A972F53F95B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14025" xr2:uid="{AA4F1BF3-BCF3-49CF-BF66-D5C4D0A0619E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="111">
   <si>
     <t>Date</t>
   </si>
@@ -352,6 +352,12 @@
   </si>
   <si>
     <t>Σ Use Case</t>
+  </si>
+  <si>
+    <t>CRUD operations fully functional for reservie tickets use case.</t>
+  </si>
+  <si>
+    <t>Added two .php files for employees to manage tickets directly via web portal</t>
   </si>
 </sst>
 </file>
@@ -805,9 +811,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B6764DD-533B-41A4-91C9-46C63E260D99}">
-  <dimension ref="A1:G53"/>
+  <dimension ref="A1:G54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
       <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
@@ -816,7 +822,7 @@
     <col min="1" max="1" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="68.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="71.7109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="70.140625" style="1" customWidth="1"/>
     <col min="6" max="6" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="41.5703125" style="1" customWidth="1"/>
@@ -1793,34 +1799,47 @@
       </c>
       <c r="G46" s="4"/>
     </row>
-    <row r="47" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="7"/>
-      <c r="B47" s="8"/>
-      <c r="C47" s="7"/>
-      <c r="D47" s="7"/>
-      <c r="E47" s="7"/>
-      <c r="F47" s="7"/>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="3">
+        <v>43108</v>
+      </c>
+      <c r="B47" s="4">
+        <v>120</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="E47" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="F47" s="4" t="s">
+        <v>9</v>
+      </c>
       <c r="G47" s="4"/>
     </row>
-    <row r="48" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="7"/>
+      <c r="B48" s="8"/>
+      <c r="C48" s="7"/>
+      <c r="D48" s="7"/>
+      <c r="E48" s="7"/>
+      <c r="F48" s="7"/>
       <c r="G48" s="4"/>
     </row>
     <row r="49" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="5" t="s">
+      <c r="G49" s="4"/>
+    </row>
+    <row r="50" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="B49" s="6">
-        <f>SUM(B2:B46)</f>
-        <v>2045</v>
-      </c>
-      <c r="C49" s="4"/>
-      <c r="D49" s="4"/>
-      <c r="E49" s="4"/>
-      <c r="F49" s="4"/>
-      <c r="G49" s="4"/>
-    </row>
-    <row r="50" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="4"/>
+      <c r="B50" s="6">
+        <f>SUM(B2:B47)</f>
+        <v>2165</v>
+      </c>
       <c r="C50" s="4"/>
       <c r="D50" s="4"/>
       <c r="E50" s="4"/>
@@ -1828,13 +1847,7 @@
       <c r="G50" s="4"/>
     </row>
     <row r="51" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="B51" s="6">
-        <f>SUM(B4:B31,B40,B43,B44,B45,B46)-B8-B19-B28-B23</f>
-        <v>1290</v>
-      </c>
+      <c r="A51" s="4"/>
       <c r="C51" s="4"/>
       <c r="D51" s="4"/>
       <c r="E51" s="4"/>
@@ -1842,18 +1855,31 @@
     </row>
     <row r="52" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B52" s="6">
-        <f>B49 -B51</f>
-        <v>755</v>
+        <f>SUM(B4:B31,B40,B43,B44,B45,B46)-B8-B19-B28-B23</f>
+        <v>1290</v>
       </c>
       <c r="C52" s="4"/>
       <c r="D52" s="4"/>
       <c r="E52" s="4"/>
       <c r="F52" s="4"/>
     </row>
-    <row r="53" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="53" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="B53" s="6">
+        <f>B50 -B52</f>
+        <v>875</v>
+      </c>
+      <c r="C53" s="4"/>
+      <c r="D53" s="4"/>
+      <c r="E53" s="4"/>
+      <c r="F53" s="4"/>
+    </row>
+    <row r="54" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>